<commit_message>
Extract numbers and dates from Excel sheets
</commit_message>
<xml_diff>
--- a/test/files/prefectures.xlsx
+++ b/test/files/prefectures.xlsx
@@ -39,9 +39,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m\月d\日"/>
+    <numFmt numFmtId="165" formatCode="yyyy/m/d\ h:mm"/>
+    <numFmt numFmtId="166" formatCode="yyyy\年mm\月dd\日"/>
+    <numFmt numFmtId="167" formatCode="m\月d\日"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -114,7 +116,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -124,6 +126,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -195,10 +205,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -218,7 +231,7 @@
       <c r="B2" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>44198</v>
       </c>
     </row>
@@ -229,7 +242,7 @@
       <c r="B3" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="4" t="n">
         <v>44199</v>
       </c>
     </row>

</xml_diff>